<commit_message>
add results by Google Colab pro plus and update parsing.py
</commit_message>
<xml_diff>
--- a/otmm_decimal/result_colab/result_existing_1000_1.0_15_40_ColabPP/a_a_1000_1.0_15_15.xlsx
+++ b/otmm_decimal/result_colab/result_existing_1000_1.0_15_40_ColabPP/a_a_1000_1.0_15_15.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\確率モデル\glycan\otmm_decimal\result_colab\result_existing_1000_1.0_15_40_ColabPP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B86A1AD4-152E-4FC3-A21D-650B750F06A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52EF6F87-84D5-4F5E-944B-B3E355895C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22560" windowHeight="14440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22560" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="a_a_1000_1.0_15_15" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -614,7 +624,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -977,11 +987,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -1697,54 +1707,54 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B17" s="2">
+      <c r="B17">
         <v>0</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17">
         <v>1</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17">
         <v>2</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17">
         <v>3</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17">
         <v>4</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17">
         <v>5</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17">
         <v>6</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17">
         <v>7</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17">
         <v>8</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K17">
         <v>9</v>
       </c>
-      <c r="L17" s="2">
+      <c r="L17">
         <v>10</v>
       </c>
-      <c r="M17" s="2">
+      <c r="M17">
         <v>11</v>
       </c>
-      <c r="N17" s="2">
+      <c r="N17">
         <v>12</v>
       </c>
-      <c r="O17" s="2">
+      <c r="O17">
         <v>13</v>
       </c>
-      <c r="P17" s="2">
+      <c r="P17">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="2">
+      <c r="A18">
         <v>0</v>
       </c>
       <c r="B18">
@@ -1809,7 +1819,7 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="2">
+      <c r="A19">
         <v>1</v>
       </c>
       <c r="B19">
@@ -1874,7 +1884,7 @@
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="2">
+      <c r="A20">
         <v>2</v>
       </c>
       <c r="B20">
@@ -1939,7 +1949,7 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="2">
+      <c r="A21">
         <v>3</v>
       </c>
       <c r="B21">
@@ -2004,7 +2014,7 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="2">
+      <c r="A22">
         <v>4</v>
       </c>
       <c r="B22">
@@ -2069,7 +2079,7 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="2">
+      <c r="A23">
         <v>5</v>
       </c>
       <c r="B23">
@@ -2134,7 +2144,7 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="2">
+      <c r="A24">
         <v>6</v>
       </c>
       <c r="B24">
@@ -2199,7 +2209,7 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="2">
+      <c r="A25">
         <v>7</v>
       </c>
       <c r="B25">
@@ -2264,7 +2274,7 @@
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="2">
+      <c r="A26">
         <v>8</v>
       </c>
       <c r="B26">
@@ -2329,7 +2339,7 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="2">
+      <c r="A27">
         <v>9</v>
       </c>
       <c r="B27">
@@ -2380,7 +2390,7 @@
         <f t="shared" si="1"/>
         <v>1.3148216172354295E-6</v>
       </c>
-      <c r="N27">
+      <c r="N27" s="2">
         <f t="shared" si="1"/>
         <v>0.12357451876924712</v>
       </c>
@@ -2394,7 +2404,7 @@
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="2">
+      <c r="A28">
         <v>10</v>
       </c>
       <c r="B28">
@@ -2459,7 +2469,7 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="2">
+      <c r="A29">
         <v>11</v>
       </c>
       <c r="B29">
@@ -2524,7 +2534,7 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="2">
+      <c r="A30">
         <v>12</v>
       </c>
       <c r="B30">
@@ -2589,7 +2599,7 @@
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="2">
+      <c r="A31">
         <v>13</v>
       </c>
       <c r="B31">
@@ -2654,7 +2664,7 @@
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="2">
+      <c r="A32">
         <v>14</v>
       </c>
       <c r="B32">

</xml_diff>